<commit_message>
Spreadsheet for vote shares
</commit_message>
<xml_diff>
--- a/chap2/vote-shares.xlsx
+++ b/chap2/vote-shares.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gheadley/CloudStation/home/school/MSc/study/MATH5872 - dissertation in data science and analytics/source/chap2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C1CBFE8-221C-6A40-B793-69410E4BC49D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AE6F28-2815-7547-ACEF-CBD3C50EABF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="460" windowWidth="34120" windowHeight="28340" xr2:uid="{18B6448F-D5E0-BE41-A3CB-6DB5FE8484F9}"/>
+    <workbookView xWindow="0" yWindow="5260" windowWidth="21600" windowHeight="28340" xr2:uid="{18B6448F-D5E0-BE41-A3CB-6DB5FE8484F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>pop totals</t>
   </si>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05D9B7C-51C3-AA4D-A4CC-9FD3AA651EF2}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="M2" sqref="M2:N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,7 +470,7 @@
     <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +489,11 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -516,8 +519,14 @@
         <f>IF(D2&gt;0.5, "circ", "sqre")</f>
         <v>circ</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -543,8 +552,14 @@
         <f t="shared" ref="G3:G37" si="3">IF(D3&gt;0.5, "circ", "sqre")</f>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -570,8 +585,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7</v>
       </c>
@@ -597,8 +618,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8</v>
       </c>
@@ -624,8 +651,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>8</v>
+      </c>
+      <c r="N6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -651,8 +684,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>13</v>
       </c>
@@ -678,8 +717,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>13</v>
+      </c>
+      <c r="N8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>14</v>
       </c>
@@ -705,8 +750,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>14</v>
+      </c>
+      <c r="N9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>15</v>
       </c>
@@ -732,8 +783,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>15</v>
+      </c>
+      <c r="N10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -759,8 +816,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -786,8 +849,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -813,8 +882,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>6</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -840,8 +915,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -867,8 +948,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>11</v>
+      </c>
+      <c r="N15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -894,8 +981,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <v>12</v>
+      </c>
+      <c r="N16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -921,8 +1014,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>16</v>
+      </c>
+      <c r="N17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -948,8 +1047,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>17</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -975,8 +1080,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>18</v>
+      </c>
+      <c r="N19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1002,8 +1113,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>19</v>
+      </c>
+      <c r="N20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1029,8 +1146,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>20</v>
+      </c>
+      <c r="N21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1056,8 +1179,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>21</v>
+      </c>
+      <c r="N22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>25</v>
       </c>
@@ -1083,8 +1212,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>25</v>
+      </c>
+      <c r="N23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>26</v>
       </c>
@@ -1110,8 +1245,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>26</v>
+      </c>
+      <c r="N24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>27</v>
       </c>
@@ -1137,8 +1278,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>27</v>
+      </c>
+      <c r="N25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>31</v>
       </c>
@@ -1164,8 +1311,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>31</v>
+      </c>
+      <c r="N26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>32</v>
       </c>
@@ -1191,8 +1344,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>32</v>
+      </c>
+      <c r="N27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>33</v>
       </c>
@@ -1218,8 +1377,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>33</v>
+      </c>
+      <c r="N28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>22</v>
       </c>
@@ -1245,8 +1410,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>22</v>
+      </c>
+      <c r="N29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>23</v>
       </c>
@@ -1272,8 +1443,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <v>23</v>
+      </c>
+      <c r="N30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>24</v>
       </c>
@@ -1299,8 +1476,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <v>24</v>
+      </c>
+      <c r="N31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1326,8 +1509,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>28</v>
+      </c>
+      <c r="N32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>29</v>
       </c>
@@ -1353,8 +1542,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>29</v>
+      </c>
+      <c r="N33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>30</v>
       </c>
@@ -1380,8 +1575,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>30</v>
+      </c>
+      <c r="N34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1407,8 +1608,14 @@
         <f t="shared" si="3"/>
         <v>circ</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <v>34</v>
+      </c>
+      <c r="N35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1434,8 +1641,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <v>35</v>
+      </c>
+      <c r="N36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1461,8 +1674,14 @@
         <f t="shared" si="3"/>
         <v>sqre</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>36</v>
+      </c>
+      <c r="N37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H39" s="3" t="s">
         <v>6</v>
       </c>
@@ -1471,7 +1690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H40" s="3" t="s">
         <v>7</v>
       </c>

</xml_diff>